<commit_message>
Indexerings -issues iets verbeterd
</commit_message>
<xml_diff>
--- a/BarcodeScanner/Prizes.xlsx
+++ b/BarcodeScanner/Prizes.xlsx
@@ -368,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A2:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -379,38 +379,38 @@
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>